<commit_message>
Modified for sugcon presentation materials
</commit_message>
<xml_diff>
--- a/DeliciousDataModel.xlsx
+++ b/DeliciousDataModel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\projects\Delicious\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E6B2726-EFFF-493F-956F-6B63C7D22361}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D572328F-09C6-4464-94DB-86430E8241D0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{E5FDF68C-D05B-43E9-BF34-15C70558D098}"/>
+    <workbookView xWindow="28680" yWindow="-1995" windowWidth="29040" windowHeight="18240" activeTab="2" xr2:uid="{E5FDF68C-D05B-43E9-BF34-15C70558D098}"/>
   </bookViews>
   <sheets>
     <sheet name="Pages" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="172">
   <si>
     <t>Feature.Events</t>
   </si>
@@ -546,6 +546,12 @@
   </si>
   <si>
     <t>Recipe Ingredient</t>
+  </si>
+  <si>
+    <t>Sitecore</t>
+  </si>
+  <si>
+    <t>Content Hub</t>
   </si>
 </sst>
 </file>
@@ -1405,10 +1411,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C51B8DD-DFA2-4D8D-8EFD-AC0C611CB301}">
-  <dimension ref="A2:P67"/>
+  <dimension ref="A1:P67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1424,6 +1430,14 @@
     <col min="13" max="13" width="40.77734375" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:16">
+      <c r="A1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F1" t="s">
+        <v>171</v>
+      </c>
+    </row>
     <row r="2" spans="1:16" ht="19.8">
       <c r="A2" t="s">
         <v>61</v>
@@ -1485,7 +1499,7 @@
       <c r="O5" s="7"/>
       <c r="P5" s="8"/>
     </row>
-    <row r="6" spans="1:16" ht="31.8" thickBot="1">
+    <row r="6" spans="1:16" ht="18" thickBot="1">
       <c r="C6" t="s">
         <v>65</v>
       </c>
@@ -1506,7 +1520,7 @@
       <c r="O6" s="7"/>
       <c r="P6" s="8"/>
     </row>
-    <row r="7" spans="1:16" ht="31.8" thickBot="1">
+    <row r="7" spans="1:16" ht="18" thickBot="1">
       <c r="C7" t="s">
         <v>66</v>
       </c>
@@ -1625,7 +1639,7 @@
       <c r="K16" s="7"/>
       <c r="L16" s="8"/>
     </row>
-    <row r="17" spans="1:16" ht="31.8" thickBot="1">
+    <row r="17" spans="1:16" ht="18" thickBot="1">
       <c r="G17" s="8"/>
       <c r="H17" s="10" t="s">
         <v>96</v>
@@ -1682,7 +1696,7 @@
       <c r="J21" s="7"/>
       <c r="K21" s="7"/>
     </row>
-    <row r="22" spans="1:16" ht="31.8" thickBot="1">
+    <row r="22" spans="1:16" ht="18" thickBot="1">
       <c r="G22" s="12"/>
       <c r="H22" s="13" t="s">
         <v>102</v>
@@ -1759,8 +1773,8 @@
       <c r="O27" s="7"/>
       <c r="P27" s="8"/>
     </row>
-    <row r="28" spans="1:16" ht="31.8" thickBot="1">
-      <c r="C28" s="10" t="s">
+    <row r="28" spans="1:16" ht="18" thickBot="1">
+      <c r="C28" s="7" t="s">
         <v>110</v>
       </c>
       <c r="G28" s="8"/>
@@ -1780,7 +1794,7 @@
       </c>
     </row>
     <row r="29" spans="1:16" ht="31.8" thickBot="1">
-      <c r="C29" s="10" t="s">
+      <c r="C29" s="7" t="s">
         <v>111</v>
       </c>
       <c r="G29" s="8"/>
@@ -1799,8 +1813,8 @@
         <v>123</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="31.8" thickBot="1">
-      <c r="C30" s="10" t="s">
+    <row r="30" spans="1:16" ht="18" thickBot="1">
+      <c r="C30" s="7" t="s">
         <v>153</v>
       </c>
       <c r="G30" s="8"/>
@@ -2179,7 +2193,7 @@
       <c r="N59" s="11"/>
       <c r="O59" s="12"/>
     </row>
-    <row r="60" spans="1:15" ht="31.8" thickBot="1">
+    <row r="60" spans="1:15" ht="18" thickBot="1">
       <c r="C60" t="s">
         <v>142</v>
       </c>
@@ -2221,7 +2235,7 @@
       <c r="K64" s="7"/>
       <c r="L64" s="8"/>
     </row>
-    <row r="65" spans="7:12" ht="31.8" thickBot="1">
+    <row r="65" spans="7:12" ht="18" thickBot="1">
       <c r="G65" s="8"/>
       <c r="H65" s="10" t="s">
         <v>143</v>

</xml_diff>